<commit_message>
BACKGROUND changes color on image click.
</commit_message>
<xml_diff>
--- a/HTML-CreativeGen.xlsx
+++ b/HTML-CreativeGen.xlsx
@@ -8,16 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miguelgarcia/Desktop/FullStack/ArtPerson/CreativePortfolio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94494725-E40E-F541-8351-E2A0A931E494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8639DA01-E280-5341-9549-F69E9167FE9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1340" yWindow="760" windowWidth="33220" windowHeight="20280" xr2:uid="{FB3A1515-A33A-8F4D-A93A-DDF6E552953B}"/>
+    <workbookView xWindow="1340" yWindow="760" windowWidth="33220" windowHeight="20180" xr2:uid="{FB3A1515-A33A-8F4D-A93A-DDF6E552953B}"/>
   </bookViews>
   <sheets>
     <sheet name="Generator" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
-    <sheet name="Generated" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="Generated" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <customWorkbookViews>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{42B17E81-1F77-D241-BD50-864917389C19}" mergeInterval="0" personalView="1" xWindow="67" yWindow="38" windowWidth="1661" windowHeight="1009" activeSheetId="1"/>
+  </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1181" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1531" uniqueCount="144">
   <si>
     <t>&lt;!--FIRST ITEM--&gt;</t>
   </si>
@@ -1281,9 +1285,6 @@
     </r>
   </si>
   <si>
-    <t>(183,3,22)</t>
-  </si>
-  <si>
     <t>AUGUST 2021</t>
   </si>
   <si>
@@ -1324,13 +1325,356 @@
   </si>
   <si>
     <t>&lt;div class="explore-middle"</t>
+  </si>
+  <si>
+    <t>&lt;div style="background-color: rgb</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">&lt;div </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>style</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="transform: translate3d(1200px, 0px, 0px)"&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>PORTO</t>
+  </si>
+  <si>
+    <t>PORTUGAL</t>
+  </si>
+  <si>
+    <t>LOVER</t>
+  </si>
+  <si>
+    <t>(13,101,56)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">&lt;li </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>style</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">="display: none" </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>index</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">="0" </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="title-1"&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>top: 49px;</t>
+  </si>
+  <si>
+    <t>height: 14px;</t>
+  </si>
+  <si>
+    <t>font-size: 12px;</t>
+  </si>
+  <si>
+    <t>line-height: 14px;</t>
+  </si>
+  <si>
+    <t>color: rgb(183, 3, 22);</t>
+  </si>
+  <si>
+    <t>transform: translate3d(101%, 0%, 0px);</t>
+  </si>
+  <si>
+    <t>opacity: 0.7;</t>
+  </si>
+  <si>
+    <t>transform: translate3d(0%, -101%, 0px);</t>
+  </si>
+  <si>
+    <t>transform: translate3d(0%, -110%, 0px);</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">&lt;li </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>style</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">="display: none" </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>index</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">="0" </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="title-2"&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">&lt;div </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>class</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">="explore line-w" </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="explore"&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>class</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="explore-top"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">&lt;div </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>style</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="background-color: rgb(183, 3, 22)"&gt;&lt;/div&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>class</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="explore-middle"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>class</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="explore-bottom"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>style</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="fill: rgb(183, 3, 22)"</t>
+    </r>
+  </si>
+  <si>
+    <t>&lt;!---END OF ITEM--&gt;</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">&lt;div </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>class</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="explore-bottom"</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1370,6 +1714,19 @@
       <color theme="1"/>
       <name val="Menlo Regular"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1391,7 +1748,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1401,6 +1758,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1715,10 +2073,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE797987-35D5-C14D-8319-D5C54AD1327E}">
-  <dimension ref="A1:N192"/>
+  <dimension ref="A1:J197"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A131" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I170" sqref="I170"/>
+    <sheetView tabSelected="1" topLeftCell="A154" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D184" sqref="D184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1734,7 +2092,7 @@
         <v>80</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>81</v>
@@ -1750,7 +2108,7 @@
     </row>
     <row r="4" spans="1:6" ht="18">
       <c r="A4" s="1" t="s">
-        <v>105</v>
+        <v>125</v>
       </c>
       <c r="B4" s="1"/>
     </row>
@@ -1812,7 +2170,7 @@
     <row r="16" spans="1:6" ht="18">
       <c r="D16" s="1" t="str">
         <f>"color: rgb"&amp;$E$1&amp;";"</f>
-        <v>color: rgb(183,3,22);</v>
+        <v>color: rgb(13,101,56);</v>
       </c>
     </row>
     <row r="17" spans="3:5" ht="18">
@@ -1832,7 +2190,7 @@
     </row>
     <row r="20" spans="3:5" ht="18">
       <c r="E20" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="3:5" ht="18">
@@ -1878,7 +2236,7 @@
     <row r="29" spans="3:5" ht="18">
       <c r="D29" s="1" t="str">
         <f>"color: rgb"&amp;$E$1&amp;";"</f>
-        <v>color: rgb(183,3,22);</v>
+        <v>color: rgb(13,101,56);</v>
       </c>
     </row>
     <row r="30" spans="3:5" ht="18">
@@ -1940,7 +2298,7 @@
       </c>
       <c r="F40" s="4" t="str">
         <f>$F$1&amp;$E$1&amp;";"</f>
-        <v>style="color: rgb(183,3,22);</v>
+        <v>style="color: rgb(13,101,56);</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>69</v>
@@ -1952,7 +2310,7 @@
     <row r="41" spans="2:8" ht="18">
       <c r="D41" s="2"/>
       <c r="E41" s="1" t="s">
-        <v>106</v>
+        <v>72</v>
       </c>
     </row>
     <row r="42" spans="2:8" ht="18">
@@ -1981,7 +2339,7 @@
       </c>
       <c r="F45" s="4" t="str">
         <f>$F$1&amp;$E$1&amp;";"</f>
-        <v>style="color: rgb(183,3,22);</v>
+        <v>style="color: rgb(13,101,56);</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>69</v>
@@ -1993,7 +2351,7 @@
     <row r="46" spans="2:8" ht="18">
       <c r="B46" s="1"/>
       <c r="E46" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
     </row>
     <row r="47" spans="2:8" ht="18">
@@ -2020,7 +2378,7 @@
       </c>
       <c r="F50" s="4" t="str">
         <f>$F$1&amp;$E$1&amp;";"</f>
-        <v>style="color: rgb(183,3,22);</v>
+        <v>style="color: rgb(13,101,56);</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>69</v>
@@ -2031,7 +2389,7 @@
     </row>
     <row r="51" spans="2:8">
       <c r="E51" t="s">
-        <v>5</v>
+        <v>90</v>
       </c>
     </row>
     <row r="52" spans="2:8" ht="18">
@@ -2060,7 +2418,7 @@
       </c>
       <c r="F55" s="4" t="str">
         <f>$F$1&amp;$E$1&amp;";"</f>
-        <v>style="color: rgb(183,3,22);</v>
+        <v>style="color: rgb(13,101,56);</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>69</v>
@@ -2072,7 +2430,7 @@
     <row r="56" spans="2:8" ht="18">
       <c r="B56" s="1"/>
       <c r="E56" t="s">
-        <v>5</v>
+        <v>106</v>
       </c>
     </row>
     <row r="57" spans="2:8" ht="18">
@@ -2102,7 +2460,7 @@
       </c>
       <c r="F60" s="4" t="str">
         <f>$F$1&amp;$E$1&amp;";"</f>
-        <v>style="color: rgb(183,3,22);</v>
+        <v>style="color: rgb(13,101,56);</v>
       </c>
       <c r="G60" s="1" t="s">
         <v>69</v>
@@ -2114,7 +2472,7 @@
     <row r="61" spans="2:8" ht="18">
       <c r="B61" s="1"/>
       <c r="E61" t="s">
-        <v>7</v>
+        <v>119</v>
       </c>
     </row>
     <row r="62" spans="2:8" ht="18">
@@ -2156,7 +2514,7 @@
       </c>
       <c r="F67" s="4" t="str">
         <f>$F$1&amp;$E$1&amp;";"</f>
-        <v>style="color: rgb(183,3,22);</v>
+        <v>style="color: rgb(13,101,56);</v>
       </c>
       <c r="G67" s="1" t="s">
         <v>76</v>
@@ -2165,7 +2523,7 @@
     <row r="68" spans="2:7" ht="18">
       <c r="B68" s="1"/>
       <c r="E68" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
     </row>
     <row r="69" spans="2:7" ht="18">
@@ -2195,7 +2553,7 @@
       </c>
       <c r="F72" s="4" t="str">
         <f>$F$1&amp;$E$1&amp;";"</f>
-        <v>style="color: rgb(183,3,22);</v>
+        <v>style="color: rgb(13,101,56);</v>
       </c>
       <c r="G72" s="1" t="s">
         <v>76</v>
@@ -2203,7 +2561,7 @@
     </row>
     <row r="73" spans="2:7">
       <c r="E73" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
     </row>
     <row r="74" spans="2:7" ht="18">
@@ -2234,7 +2592,7 @@
       </c>
       <c r="F77" s="4" t="str">
         <f>$F$1&amp;$E$1&amp;";"</f>
-        <v>style="color: rgb(183,3,22);</v>
+        <v>style="color: rgb(13,101,56);</v>
       </c>
       <c r="G77" s="1" t="s">
         <v>76</v>
@@ -2243,7 +2601,7 @@
     <row r="78" spans="2:7" ht="18">
       <c r="B78" s="1"/>
       <c r="E78" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="79" spans="2:7" ht="18">
@@ -2274,7 +2632,7 @@
       </c>
       <c r="F82" s="4" t="str">
         <f>$F$1&amp;$E$1&amp;";"</f>
-        <v>style="color: rgb(183,3,22);</v>
+        <v>style="color: rgb(13,101,56);</v>
       </c>
       <c r="G82" s="1" t="s">
         <v>76</v>
@@ -2283,7 +2641,7 @@
     <row r="83" spans="2:7" ht="18">
       <c r="B83" s="1"/>
       <c r="E83" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
     </row>
     <row r="84" spans="2:7" ht="18">
@@ -2301,7 +2659,7 @@
     <row r="86" spans="2:7" ht="18">
       <c r="B86" s="1"/>
       <c r="C86" s="1" t="s">
-        <v>49</v>
+        <v>120</v>
       </c>
     </row>
     <row r="87" spans="2:7" ht="18">
@@ -2314,7 +2672,7 @@
       </c>
       <c r="F87" s="4" t="str">
         <f>$F$1&amp;$E$1&amp;";"</f>
-        <v>style="color: rgb(183,3,22);</v>
+        <v>style="color: rgb(13,101,56);</v>
       </c>
       <c r="G87" s="1" t="s">
         <v>76</v>
@@ -2323,7 +2681,7 @@
     <row r="88" spans="2:7" ht="18">
       <c r="B88" s="1"/>
       <c r="E88" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="89" spans="2:7" ht="18">
@@ -2339,123 +2697,121 @@
       </c>
     </row>
     <row r="91" spans="2:7" ht="18">
-      <c r="B91" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C91" s="2" t="s">
+      <c r="B91" s="1"/>
+      <c r="C91" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="92" spans="2:7" ht="18">
+      <c r="B92" s="1"/>
+      <c r="D92" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F92" s="4" t="str">
+        <f>$F$1&amp;$E$1&amp;";"</f>
+        <v>style="color: rgb(13,101,56);</v>
+      </c>
+      <c r="G92" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="93" spans="2:7" ht="18">
+      <c r="B93" s="1"/>
+      <c r="E93" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="94" spans="2:7" ht="18">
+      <c r="B94" s="1"/>
+      <c r="D94" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="95" spans="2:7" ht="18">
+      <c r="B95" s="1"/>
+      <c r="C95" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="96" spans="2:7" ht="18">
+      <c r="B96" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C96" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="2:7" ht="18">
-      <c r="B92" s="2"/>
-    </row>
-    <row r="93" spans="2:7" ht="18">
-      <c r="B93" s="1" t="s">
+    <row r="97" spans="2:7" ht="18">
+      <c r="B97" s="2"/>
+    </row>
+    <row r="98" spans="2:7" ht="18">
+      <c r="B98" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="94" spans="2:7" ht="18">
-      <c r="C94" s="1" t="s">
+    <row r="99" spans="2:7" ht="18">
+      <c r="C99" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D94" s="2" t="s">
+      <c r="D99" s="2" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="95" spans="2:7" ht="18">
-      <c r="D95" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E95" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F95" s="4" t="str">
-        <f>$F$1&amp;$E$1&amp;";"</f>
-        <v>style="color: rgb(183,3,22);</v>
-      </c>
-      <c r="G95" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="96" spans="2:7" ht="18">
-      <c r="E96" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="97" spans="2:7" ht="18">
-      <c r="D97" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="98" spans="2:7" ht="18">
-      <c r="D98" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E98" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F98" s="4" t="str">
-        <f>$F$1&amp;$E$1&amp;";"</f>
-        <v>style="color: rgb(183,3,22);</v>
-      </c>
-      <c r="G98" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="99" spans="2:7" ht="18">
-      <c r="E99" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="100" spans="2:7" ht="18">
       <c r="D100" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F100" s="4" t="str">
+        <f>$F$1&amp;$E$1&amp;";"</f>
+        <v>style="color: rgb(13,101,56);</v>
+      </c>
+      <c r="G100" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="101" spans="2:7" ht="18">
-      <c r="B101" s="1"/>
-      <c r="D101" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E101" s="2" t="s">
+      <c r="E101" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="2:7" ht="18">
+      <c r="D102" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="103" spans="2:7" ht="18">
+      <c r="D103" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E103" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F101" s="4" t="str">
-        <f>$F$1&amp;$E$1&amp;";"</f>
-        <v>style="color: rgb(183,3,22);</v>
-      </c>
-      <c r="G101" s="1" t="s">
+      <c r="F103" s="4" t="str">
+        <f>$F$1&amp;$E$1&amp;";"</f>
+        <v>style="color: rgb(13,101,56);</v>
+      </c>
+      <c r="G103" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="102" spans="2:7" ht="18">
-      <c r="B102" s="1"/>
-      <c r="E102" s="7" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="103" spans="2:7" ht="18">
-      <c r="B103" s="1"/>
-      <c r="D103" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
     <row r="104" spans="2:7" ht="18">
-      <c r="B104" s="1"/>
-      <c r="C104" s="1" t="s">
-        <v>34</v>
+      <c r="E104" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="105" spans="2:7" ht="18">
-      <c r="B105" s="1"/>
-      <c r="C105" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D105" s="2" t="s">
-        <v>12</v>
+      <c r="D105" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="106" spans="2:7" ht="18">
+      <c r="B106" s="1"/>
       <c r="D106" s="1" t="s">
         <v>28</v>
       </c>
@@ -2464,15 +2820,16 @@
       </c>
       <c r="F106" s="4" t="str">
         <f>$F$1&amp;$E$1&amp;";"</f>
-        <v>style="color: rgb(183,3,22);</v>
+        <v>style="color: rgb(13,101,56);</v>
       </c>
       <c r="G106" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="107" spans="2:7" ht="18">
-      <c r="E107" s="1">
-        <v>2</v>
+      <c r="B107" s="1"/>
+      <c r="E107" s="7" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="108" spans="2:7" ht="18">
@@ -2482,74 +2839,72 @@
       </c>
     </row>
     <row r="109" spans="2:7" ht="18">
-      <c r="B109" s="2"/>
-      <c r="D109" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E109" s="2" t="s">
+      <c r="B109" s="1"/>
+      <c r="C109" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="110" spans="2:7" ht="18">
+      <c r="B110" s="1"/>
+      <c r="C110" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="111" spans="2:7" ht="18">
+      <c r="D111" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E111" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F109" s="4" t="str">
-        <f>$F$1&amp;$E$1&amp;";"</f>
-        <v>style="color: rgb(183,3,22);</v>
-      </c>
-      <c r="G109" s="1" t="s">
+      <c r="F111" s="4" t="str">
+        <f>$F$1&amp;$E$1&amp;";"</f>
+        <v>style="color: rgb(13,101,56);</v>
+      </c>
+      <c r="G111" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="110" spans="2:7" ht="18">
-      <c r="B110" s="2"/>
-      <c r="E110" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="111" spans="2:7" ht="18">
-      <c r="B111" s="1"/>
-      <c r="D111" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
     <row r="112" spans="2:7" ht="18">
-      <c r="B112" s="1"/>
-      <c r="D112" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E112" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F112" s="4" t="str">
-        <f>$F$1&amp;$E$1&amp;";"</f>
-        <v>style="color: rgb(183,3,22);</v>
-      </c>
-      <c r="G112" s="1" t="s">
-        <v>77</v>
+      <c r="E112" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="113" spans="2:7" ht="18">
       <c r="B113" s="1"/>
-      <c r="E113" s="3" t="s">
-        <v>113</v>
+      <c r="D113" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="114" spans="2:7" ht="18">
-      <c r="B114" s="1"/>
+      <c r="B114" s="2"/>
       <c r="D114" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
+      </c>
+      <c r="E114" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F114" s="4" t="str">
+        <f>$F$1&amp;$E$1&amp;";"</f>
+        <v>style="color: rgb(13,101,56);</v>
+      </c>
+      <c r="G114" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="115" spans="2:7" ht="18">
-      <c r="B115" s="1"/>
-      <c r="C115" s="1" t="s">
-        <v>34</v>
+      <c r="B115" s="2"/>
+      <c r="E115" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="116" spans="2:7" ht="18">
       <c r="B116" s="1"/>
-      <c r="C116" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D116" s="2" t="s">
-        <v>14</v>
+      <c r="D116" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="117" spans="2:7" ht="18">
@@ -2562,7 +2917,7 @@
       </c>
       <c r="F117" s="4" t="str">
         <f>$F$1&amp;$E$1&amp;";"</f>
-        <v>style="color: rgb(183,3,22);</v>
+        <v>style="color: rgb(13,101,56);</v>
       </c>
       <c r="G117" s="1" t="s">
         <v>77</v>
@@ -2570,85 +2925,85 @@
     </row>
     <row r="118" spans="2:7" ht="18">
       <c r="B118" s="1"/>
-      <c r="E118" s="1">
-        <v>3</v>
+      <c r="E118" s="3" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="119" spans="2:7" ht="18">
-      <c r="B119" s="2"/>
+      <c r="B119" s="1"/>
       <c r="D119" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="120" spans="2:7" ht="18">
-      <c r="B120" s="2"/>
-      <c r="D120" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E120" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F120" s="4" t="str">
-        <f>$F$1&amp;$E$1&amp;";"</f>
-        <v>style="color: rgb(183,3,22);</v>
-      </c>
-      <c r="G120" s="1" t="s">
-        <v>77</v>
+      <c r="B120" s="1"/>
+      <c r="C120" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="121" spans="2:7" ht="18">
       <c r="B121" s="1"/>
-      <c r="E121" s="1" t="s">
-        <v>15</v>
+      <c r="C121" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D121" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="122" spans="2:7" ht="18">
       <c r="B122" s="1"/>
       <c r="D122" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
+      </c>
+      <c r="E122" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F122" s="4" t="str">
+        <f>$F$1&amp;$E$1&amp;";"</f>
+        <v>style="color: rgb(13,101,56);</v>
+      </c>
+      <c r="G122" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="123" spans="2:7" ht="18">
       <c r="B123" s="1"/>
-      <c r="D123" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E123" s="2" t="s">
+      <c r="E123" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="124" spans="2:7" ht="18">
+      <c r="B124" s="2"/>
+      <c r="D124" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="125" spans="2:7" ht="18">
+      <c r="B125" s="2"/>
+      <c r="D125" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E125" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F123" s="4" t="str">
-        <f>$F$1&amp;$E$1&amp;";"</f>
-        <v>style="color: rgb(183,3,22);</v>
-      </c>
-      <c r="G123" s="1" t="s">
+      <c r="F125" s="4" t="str">
+        <f>$F$1&amp;$E$1&amp;";"</f>
+        <v>style="color: rgb(13,101,56);</v>
+      </c>
+      <c r="G125" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="124" spans="2:7" ht="18">
-      <c r="B124" s="1"/>
-      <c r="E124" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="125" spans="2:7" ht="18">
-      <c r="B125" s="1"/>
-      <c r="D125" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
     <row r="126" spans="2:7" ht="18">
-      <c r="B126" s="3"/>
-      <c r="C126" s="1" t="s">
-        <v>34</v>
+      <c r="B126" s="1"/>
+      <c r="E126" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="127" spans="2:7" ht="18">
       <c r="B127" s="1"/>
-      <c r="C127" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D127" s="2" t="s">
-        <v>16</v>
+      <c r="D127" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="128" spans="2:7" ht="18">
@@ -2661,7 +3016,7 @@
       </c>
       <c r="F128" s="4" t="str">
         <f>$F$1&amp;$E$1&amp;";"</f>
-        <v>style="color: rgb(183,3,22);</v>
+        <v>style="color: rgb(13,101,56);</v>
       </c>
       <c r="G128" s="1" t="s">
         <v>77</v>
@@ -2669,140 +3024,145 @@
     </row>
     <row r="129" spans="2:7" ht="18">
       <c r="B129" s="1"/>
-      <c r="E129" s="1">
-        <v>4</v>
+      <c r="E129" s="3" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="130" spans="2:7" ht="18">
-      <c r="B130" s="2"/>
+      <c r="B130" s="1"/>
       <c r="D130" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="131" spans="2:7" ht="18">
-      <c r="B131" s="1"/>
-      <c r="D131" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E131" s="2" t="s">
+      <c r="B131" s="3"/>
+      <c r="C131" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="132" spans="2:7" ht="18">
+      <c r="B132" s="1"/>
+      <c r="C132" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D132" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="133" spans="2:7" ht="18">
+      <c r="B133" s="1"/>
+      <c r="D133" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E133" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F131" s="4" t="str">
-        <f>$F$1&amp;$E$1&amp;";"</f>
-        <v>style="color: rgb(183,3,22);</v>
-      </c>
-      <c r="G131" s="1" t="s">
+      <c r="F133" s="4" t="str">
+        <f>$F$1&amp;$E$1&amp;";"</f>
+        <v>style="color: rgb(13,101,56);</v>
+      </c>
+      <c r="G133" s="1" t="s">
         <v>77</v>
-      </c>
-    </row>
-    <row r="132" spans="2:7" ht="18">
-      <c r="B132" s="2"/>
-      <c r="E132" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="133" spans="2:7" ht="18">
-      <c r="B133" s="2"/>
-      <c r="D133" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="134" spans="2:7" ht="18">
       <c r="B134" s="1"/>
-      <c r="D134" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E134" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F134" s="4" t="str">
-        <f>$F$1&amp;$E$1&amp;";"</f>
-        <v>style="color: rgb(183,3,22);</v>
-      </c>
-      <c r="G134" s="1" t="s">
-        <v>77</v>
+      <c r="E134" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="135" spans="2:7" ht="18">
-      <c r="B135" s="1"/>
-      <c r="E135" s="3" t="s">
-        <v>115</v>
+      <c r="B135" s="2"/>
+      <c r="D135" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="136" spans="2:7" ht="18">
       <c r="B136" s="1"/>
       <c r="D136" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
+      </c>
+      <c r="E136" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F136" s="4" t="str">
+        <f>$F$1&amp;$E$1&amp;";"</f>
+        <v>style="color: rgb(13,101,56);</v>
+      </c>
+      <c r="G136" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="137" spans="2:7" ht="18">
-      <c r="B137" s="1"/>
-      <c r="C137" s="1" t="s">
-        <v>34</v>
+      <c r="B137" s="2"/>
+      <c r="E137" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="138" spans="2:7" ht="18">
-      <c r="B138" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C138" s="2" t="s">
+      <c r="B138" s="2"/>
+      <c r="D138" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="139" spans="2:7" ht="18">
+      <c r="B139" s="1"/>
+      <c r="D139" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E139" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F139" s="4" t="str">
+        <f>$F$1&amp;$E$1&amp;";"</f>
+        <v>style="color: rgb(13,101,56);</v>
+      </c>
+      <c r="G139" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="140" spans="2:7" ht="18">
+      <c r="B140" s="1"/>
+      <c r="E140" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="141" spans="2:7" ht="18">
+      <c r="B141" s="1"/>
+      <c r="D141" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="142" spans="2:7" ht="18">
+      <c r="B142" s="1"/>
+      <c r="C142" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="143" spans="2:7" ht="18">
+      <c r="B143" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C143" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="139" spans="2:7" ht="18">
-      <c r="B139" s="1" t="s">
+    <row r="144" spans="2:7" ht="18">
+      <c r="B144" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="140" spans="2:7" ht="18">
-      <c r="B140" s="2"/>
-      <c r="C140" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D140" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F140" s="4"/>
-    </row>
-    <row r="141" spans="2:7" ht="18">
-      <c r="D141" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E141" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F141" s="4" t="str">
-        <f>$F$1&amp;$E$1&amp;";"</f>
-        <v>style="color: rgb(183,3,22);</v>
-      </c>
-      <c r="G141" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="142" spans="2:7" ht="18">
-      <c r="E142" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="143" spans="2:7" ht="18">
-      <c r="D143" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="144" spans="2:7" ht="18">
-      <c r="C144" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="145" spans="2:14" ht="18">
+    <row r="145" spans="2:7" ht="18">
+      <c r="B145" s="2"/>
       <c r="C145" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="146" spans="2:14" ht="18">
+        <v>10</v>
+      </c>
+      <c r="F145" s="4"/>
+    </row>
+    <row r="146" spans="2:7" ht="18">
       <c r="D146" s="1" t="s">
         <v>28</v>
       </c>
@@ -2811,304 +3171,2111 @@
       </c>
       <c r="F146" s="4" t="str">
         <f>$F$1&amp;$E$1&amp;";"</f>
-        <v>style="color: rgb(183,3,22);</v>
+        <v>style="color: rgb(13,101,56);</v>
       </c>
       <c r="G146" s="6" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="147" spans="2:14" ht="18">
+    <row r="147" spans="2:7" ht="18">
       <c r="E147" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="148" spans="2:7" ht="18">
+      <c r="D148" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="149" spans="2:7" ht="18">
+      <c r="C149" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="150" spans="2:7" ht="18">
+      <c r="C150" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D150" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="151" spans="2:7" ht="18">
+      <c r="D151" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E151" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F151" s="4" t="str">
+        <f>$F$1&amp;$E$1&amp;";"</f>
+        <v>style="color: rgb(13,101,56);</v>
+      </c>
+      <c r="G151" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="152" spans="2:7" ht="18">
+      <c r="E152" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="148" spans="2:14" ht="18">
-      <c r="D148" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="149" spans="2:14" ht="18">
-      <c r="C149" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="150" spans="2:14" ht="18">
-      <c r="B150" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C150" s="2" t="s">
+    <row r="153" spans="2:7" ht="18">
+      <c r="D153" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="154" spans="2:7" ht="18">
+      <c r="C154" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="155" spans="2:7" ht="18">
+      <c r="B155" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C155" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="152" spans="2:14" ht="18">
-      <c r="B152" s="1" t="s">
+    <row r="157" spans="2:7" ht="18">
+      <c r="B157" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="158" spans="2:7" ht="18">
+      <c r="C158" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D158" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="159" spans="2:7" ht="18">
+      <c r="D159" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="153" spans="2:14" ht="18">
-      <c r="C153" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E153" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="154" spans="2:14" ht="18">
-      <c r="D154" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="E154" s="4" t="str">
-        <f>$F$1&amp;$E$1&amp;";"</f>
-        <v>style="color: rgb(183,3,22);</v>
-      </c>
-      <c r="F154" s="6" t="s">
+      <c r="E159" s="4" t="str">
+        <f>$F$1&amp;$E$1&amp;";"</f>
+        <v>style="color: rgb(13,101,56);</v>
+      </c>
+      <c r="F159" s="6" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="155" spans="2:14" ht="18">
-      <c r="E155" s="1" t="s">
+    <row r="160" spans="2:7" ht="18">
+      <c r="E160" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="156" spans="2:14" ht="18">
-      <c r="B156" s="2"/>
-      <c r="F156" s="1" t="s">
+    <row r="161" spans="2:10" ht="18">
+      <c r="B161" s="2"/>
+      <c r="F161" s="1" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="157" spans="2:14" ht="18">
-      <c r="B157" s="1"/>
-      <c r="G157" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="L157" s="6" t="str">
-        <f>$E$1</f>
-        <v>(183,3,22)</v>
-      </c>
-      <c r="M157" t="s">
-        <v>3</v>
-      </c>
-      <c r="N157" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="158" spans="2:14" ht="18">
-      <c r="B158" s="1"/>
-      <c r="G158" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="L158" s="6" t="str">
-        <f>$E$1</f>
-        <v>(183,3,22)</v>
-      </c>
-      <c r="M158" t="s">
-        <v>3</v>
-      </c>
-      <c r="N158" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="159" spans="2:14" ht="18">
-      <c r="B159" s="1"/>
-      <c r="F159" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="160" spans="2:14" ht="18">
-      <c r="B160" s="1"/>
-      <c r="E160" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="161" spans="2:10" ht="18">
-      <c r="B161" s="1"/>
-      <c r="D161" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="162" spans="2:10" ht="18">
       <c r="B162" s="1"/>
-      <c r="C162" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E162" s="2" t="s">
-        <v>25</v>
+      <c r="G162" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H162" s="6" t="str">
+        <f>$E$1</f>
+        <v>(13,101,56)</v>
+      </c>
+      <c r="I162" t="s">
+        <v>3</v>
+      </c>
+      <c r="J162" s="6" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="163" spans="2:10" ht="18">
       <c r="B163" s="1"/>
-      <c r="D163" s="1" t="s">
+      <c r="G163" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="E163" s="4" t="str">
-        <f>$F$1&amp;$E$1&amp;";"</f>
-        <v>style="color: rgb(183,3,22);</v>
-      </c>
-      <c r="F163" s="6" t="s">
-        <v>84</v>
+      <c r="H163" s="6" t="str">
+        <f>$E$1</f>
+        <v>(13,101,56)</v>
+      </c>
+      <c r="I163" t="s">
+        <v>3</v>
+      </c>
+      <c r="J163" s="6" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="164" spans="2:10" ht="18">
       <c r="B164" s="1"/>
-      <c r="D164" t="s">
-        <v>34</v>
-      </c>
-      <c r="F164" s="6"/>
+      <c r="F164" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="165" spans="2:10" ht="18">
       <c r="B165" s="1"/>
-      <c r="C165" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F165" s="6"/>
+      <c r="D165" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="166" spans="2:10" ht="18">
+      <c r="B166" s="1"/>
       <c r="C166" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E166" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F166" s="4"/>
-    </row>
-    <row r="167" spans="2:10" ht="18">
-      <c r="B167" s="1"/>
-      <c r="D167" s="1"/>
-      <c r="E167" s="4" t="str">
-        <f>$F$1&amp;$E$1&amp;";"</f>
-        <v>style="color: rgb(183,3,22);</v>
-      </c>
-      <c r="F167" s="6" t="s">
-        <v>84</v>
+        <v>34</v>
       </c>
     </row>
     <row r="168" spans="2:10" ht="18">
       <c r="B168" s="1"/>
-      <c r="E168" s="1" t="s">
-        <v>61</v>
+      <c r="C168" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E168" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="169" spans="2:10" ht="18">
-      <c r="F169" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G169" s="2" t="s">
-        <v>63</v>
+      <c r="B169" s="1"/>
+      <c r="D169" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E169" s="4" t="str">
+        <f>$F$1&amp;$E$1&amp;";"</f>
+        <v>style="color: rgb(13,101,56);</v>
+      </c>
+      <c r="F169" s="6" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="170" spans="2:10" ht="18">
-      <c r="G170" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="H170" s="6" t="str">
-        <f>$E$1</f>
-        <v>(183,3,22)</v>
-      </c>
-      <c r="I170" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="J170" s="6"/>
+      <c r="B170" s="1"/>
+      <c r="D170" t="s">
+        <v>34</v>
+      </c>
+      <c r="F170" s="6"/>
     </row>
     <row r="171" spans="2:10" ht="18">
       <c r="B171" s="1"/>
-      <c r="G171" s="2" t="s">
-        <v>64</v>
-      </c>
+      <c r="C171" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F171" s="6"/>
     </row>
     <row r="172" spans="2:10" ht="18">
-      <c r="B172" s="2"/>
-      <c r="F172" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G172" s="2"/>
+      <c r="C172" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E172" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F172" s="4"/>
     </row>
     <row r="173" spans="2:10" ht="18">
       <c r="B173" s="1"/>
-      <c r="E173" s="1" t="s">
-        <v>66</v>
+      <c r="D173" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="E173" s="4" t="str">
+        <f>$F$1&amp;$E$1&amp;";"</f>
+        <v>style="color: rgb(13,101,56);</v>
+      </c>
+      <c r="F173" s="6" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="174" spans="2:10" ht="18">
       <c r="B174" s="1"/>
-      <c r="D174" s="1" t="s">
-        <v>34</v>
+      <c r="E174" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="175" spans="2:10" ht="18">
-      <c r="B175" s="1"/>
-      <c r="C175" s="1" t="s">
-        <v>34</v>
+      <c r="F175" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G175" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="176" spans="2:10" ht="18">
-      <c r="B176" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C176" s="2" t="s">
+      <c r="G176" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H176" s="6" t="str">
+        <f>$E$1</f>
+        <v>(13,101,56)</v>
+      </c>
+      <c r="I176" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J176" s="6"/>
+    </row>
+    <row r="177" spans="1:7" ht="18">
+      <c r="B177" s="1"/>
+      <c r="G177" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" ht="18">
+      <c r="B178" s="2"/>
+      <c r="F178" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G178" s="2"/>
+    </row>
+    <row r="179" spans="1:7" ht="18">
+      <c r="B179" s="1"/>
+      <c r="E179" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" ht="18">
+      <c r="B180" s="1"/>
+      <c r="D180" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" ht="18">
+      <c r="B181" s="1"/>
+      <c r="C181" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" ht="18">
+      <c r="B182" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C182" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="177" spans="1:1" ht="18">
-      <c r="A177" s="1" t="s">
+    <row r="183" spans="1:7" ht="18">
+      <c r="A183" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="178" spans="1:1" ht="18">
-      <c r="A178" s="1"/>
-    </row>
-    <row r="179" spans="1:1" ht="18">
-      <c r="A179" s="2"/>
-    </row>
-    <row r="180" spans="1:1" ht="18">
-      <c r="A180" s="1"/>
-    </row>
-    <row r="181" spans="1:1" ht="18">
-      <c r="A181" s="1"/>
-    </row>
-    <row r="182" spans="1:1" ht="18">
-      <c r="A182" s="1"/>
-    </row>
-    <row r="183" spans="1:1" ht="18">
-      <c r="A183" s="2"/>
-    </row>
-    <row r="184" spans="1:1" ht="18">
-      <c r="A184" s="2"/>
-    </row>
-    <row r="185" spans="1:1" ht="18">
+      <c r="B183" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" ht="18">
+      <c r="A184" s="1"/>
+    </row>
+    <row r="185" spans="1:7" ht="18">
       <c r="A185" s="2"/>
     </row>
-    <row r="186" spans="1:1" ht="18">
+    <row r="186" spans="1:7" ht="18">
       <c r="A186" s="1"/>
     </row>
-    <row r="187" spans="1:1" ht="18">
+    <row r="187" spans="1:7" ht="18">
       <c r="A187" s="1"/>
     </row>
-    <row r="188" spans="1:1" ht="18">
-      <c r="A188" s="1"/>
-    </row>
-    <row r="189" spans="1:1" ht="18">
-      <c r="A189" s="1"/>
-    </row>
-    <row r="190" spans="1:1" ht="18">
-      <c r="A190" s="1"/>
-    </row>
-    <row r="191" spans="1:1" ht="18">
-      <c r="A191" s="2"/>
-    </row>
-    <row r="192" spans="1:1" ht="18">
+    <row r="188" spans="1:7" ht="18">
+      <c r="A188" s="2"/>
+    </row>
+    <row r="189" spans="1:7" ht="18">
+      <c r="A189" s="2"/>
+    </row>
+    <row r="190" spans="1:7" ht="18">
+      <c r="A190" s="2"/>
+    </row>
+    <row r="191" spans="1:7" ht="18">
+      <c r="A191" s="1"/>
+    </row>
+    <row r="192" spans="1:7" ht="18">
       <c r="A192" s="1"/>
     </row>
+    <row r="193" spans="1:1" ht="18">
+      <c r="A193" s="1"/>
+    </row>
+    <row r="194" spans="1:1" ht="18">
+      <c r="A194" s="1"/>
+    </row>
+    <row r="195" spans="1:1" ht="18">
+      <c r="A195" s="1"/>
+    </row>
+    <row r="196" spans="1:1" ht="18">
+      <c r="A196" s="2"/>
+    </row>
+    <row r="197" spans="1:1" ht="18">
+      <c r="A197" s="1"/>
+    </row>
   </sheetData>
+  <customSheetViews>
+    <customSheetView guid="{42B17E81-1F77-D241-BD50-864917389C19}" scale="70" topLeftCell="A149">
+      <selection activeCell="D177" sqref="D177"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+  </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5222863-6D48-3346-BD80-2256CF923EA2}">
+  <dimension ref="A3:B352"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F329" sqref="F329"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="3" spans="1:2" ht="18">
+      <c r="A3" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="18">
+      <c r="B4" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="18">
+      <c r="B5" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="18">
+      <c r="B6" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="18">
+      <c r="B7" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="18">
+      <c r="B8" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="18">
+      <c r="B9" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="18">
+      <c r="B10" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="18">
+      <c r="B11" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="18">
+      <c r="B12" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="18">
+      <c r="B13" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="18">
+      <c r="B14" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="18">
+      <c r="B15" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="18">
+      <c r="B16" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" ht="18">
+      <c r="B17" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" ht="18">
+      <c r="B18" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" ht="18">
+      <c r="B19" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" ht="18">
+      <c r="B20" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" ht="18">
+      <c r="B21" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" ht="18">
+      <c r="B22" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" ht="18">
+      <c r="B23" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" ht="18">
+      <c r="B24" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" ht="18">
+      <c r="B25" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" ht="18">
+      <c r="B26" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" ht="18">
+      <c r="B27" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" ht="18">
+      <c r="B28" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" ht="18">
+      <c r="B29" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" ht="18">
+      <c r="B30" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" ht="18">
+      <c r="B31" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2" ht="18">
+      <c r="B32" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" ht="18">
+      <c r="B33" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" ht="18">
+      <c r="B34" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" ht="18">
+      <c r="B35" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" ht="18">
+      <c r="B36" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" ht="18">
+      <c r="B37" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" ht="18">
+      <c r="B38" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" ht="18">
+      <c r="B39" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" ht="18">
+      <c r="B40" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" ht="18">
+      <c r="B41" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2" ht="18">
+      <c r="B42" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2" ht="18">
+      <c r="B43" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2" ht="18">
+      <c r="B44" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2" ht="18">
+      <c r="B45" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2" ht="18">
+      <c r="B46" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2" ht="18">
+      <c r="B47" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2" ht="18">
+      <c r="B48" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" ht="18">
+      <c r="B49" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" ht="18">
+      <c r="B50" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" ht="18">
+      <c r="B51" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" ht="18">
+      <c r="B52" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" ht="18">
+      <c r="B53" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" ht="18">
+      <c r="B54" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2" ht="18">
+      <c r="B55" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2" ht="18">
+      <c r="B56" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2" ht="18">
+      <c r="B57" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2" ht="18">
+      <c r="B58" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2" ht="18">
+      <c r="B59" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2" ht="18">
+      <c r="B60" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="2:2" ht="18">
+      <c r="B61" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="2:2" ht="18">
+      <c r="B62" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="63" spans="2:2" ht="18">
+      <c r="B63" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="64" spans="2:2" ht="18">
+      <c r="B64" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" ht="18">
+      <c r="B65" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" ht="18">
+      <c r="B66" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" ht="18">
+      <c r="B67" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2" ht="18">
+      <c r="B68" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2" ht="18">
+      <c r="B69" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2" ht="18">
+      <c r="B70" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2" ht="18">
+      <c r="B71" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2" ht="18">
+      <c r="B72" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2" ht="18">
+      <c r="B73" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="2:2" ht="18">
+      <c r="B74" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="75" spans="2:2" ht="18">
+      <c r="B75" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="76" spans="2:2" ht="18">
+      <c r="B76" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="77" spans="2:2" ht="18">
+      <c r="B77" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="78" spans="2:2" ht="18">
+      <c r="B78" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="79" spans="2:2" ht="18">
+      <c r="B79" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="80" spans="2:2" ht="18">
+      <c r="B80" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2" ht="18">
+      <c r="B81" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2" ht="18">
+      <c r="B82" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2" ht="18">
+      <c r="B83" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="84" spans="2:2" ht="18">
+      <c r="B84" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="85" spans="2:2" ht="18">
+      <c r="B85" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86" spans="2:2" ht="18">
+      <c r="B86" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="2:2" ht="18">
+      <c r="B87" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="88" spans="2:2" ht="18">
+      <c r="B88" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="89" spans="2:2" ht="18">
+      <c r="B89" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="90" spans="2:2" ht="18">
+      <c r="B90" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="91" spans="2:2" ht="18">
+      <c r="B91" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="92" spans="2:2" ht="18">
+      <c r="B92" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="93" spans="2:2" ht="18">
+      <c r="B93" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="94" spans="2:2" ht="18">
+      <c r="B94" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="95" spans="2:2" ht="18">
+      <c r="B95" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="96" spans="2:2" ht="18">
+      <c r="B96" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2" ht="18">
+      <c r="B97" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="2:2" ht="18">
+      <c r="B98" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="99" spans="2:2" ht="18">
+      <c r="B99" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="100" spans="2:2" ht="18">
+      <c r="B100" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="101" spans="2:2" ht="18">
+      <c r="B101" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="102" spans="2:2" ht="18">
+      <c r="B102" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="103" spans="2:2" ht="18">
+      <c r="B103" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="104" spans="2:2" ht="18">
+      <c r="B104" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="105" spans="2:2" ht="18">
+      <c r="B105" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="106" spans="2:2" ht="18">
+      <c r="B106" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="107" spans="2:2" ht="18">
+      <c r="B107" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="108" spans="2:2" ht="18">
+      <c r="B108" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="2:2" ht="18">
+      <c r="B109" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="110" spans="2:2" ht="18">
+      <c r="B110" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="111" spans="2:2" ht="18">
+      <c r="B111" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="112" spans="2:2" ht="18">
+      <c r="B112" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="113" spans="2:2" ht="18">
+      <c r="B113" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="114" spans="2:2" ht="18">
+      <c r="B114" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="115" spans="2:2" ht="18">
+      <c r="B115" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="116" spans="2:2" ht="18">
+      <c r="B116" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="117" spans="2:2" ht="18">
+      <c r="B117" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="118" spans="2:2" ht="18">
+      <c r="B118" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="119" spans="2:2" ht="18">
+      <c r="B119" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="2:2" ht="18">
+      <c r="B120" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="121" spans="2:2" ht="18">
+      <c r="B121" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="122" spans="2:2" ht="18">
+      <c r="B122" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="123" spans="2:2" ht="18">
+      <c r="B123" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="124" spans="2:2" ht="18">
+      <c r="B124" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="125" spans="2:2" ht="18">
+      <c r="B125" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="126" spans="2:2" ht="18">
+      <c r="B126" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="127" spans="2:2" ht="18">
+      <c r="B127" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="128" spans="2:2" ht="18">
+      <c r="B128" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="129" spans="2:2" ht="18">
+      <c r="B129" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="130" spans="2:2" ht="18">
+      <c r="B130" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="2:2" ht="18">
+      <c r="B131" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="132" spans="2:2" ht="18">
+      <c r="B132" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="133" spans="2:2" ht="18">
+      <c r="B133" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="134" spans="2:2" ht="18">
+      <c r="B134" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="135" spans="2:2" ht="18">
+      <c r="B135" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="137" spans="2:2" ht="18">
+      <c r="B137" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="138" spans="2:2" ht="18">
+      <c r="B138" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="139" spans="2:2" ht="18">
+      <c r="B139" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="140" spans="2:2" ht="18">
+      <c r="B140" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="141" spans="2:2" ht="18">
+      <c r="B141" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="142" spans="2:2" ht="18">
+      <c r="B142" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="143" spans="2:2" ht="18">
+      <c r="B143" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="144" spans="2:2" ht="18">
+      <c r="B144" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="145" spans="2:2" ht="18">
+      <c r="B145" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="146" spans="2:2" ht="18">
+      <c r="B146" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="147" spans="2:2" ht="18">
+      <c r="B147" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="2:2" ht="18">
+      <c r="B148" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="2:2" ht="18">
+      <c r="B149" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="150" spans="2:2" ht="18">
+      <c r="B150" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="151" spans="2:2" ht="18">
+      <c r="B151" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="152" spans="2:2" ht="18">
+      <c r="B152" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="153" spans="2:2" ht="18">
+      <c r="B153" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="154" spans="2:2" ht="18">
+      <c r="B154" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="155" spans="2:2" ht="18">
+      <c r="B155" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="156" spans="2:2" ht="18">
+      <c r="B156" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="157" spans="2:2" ht="18">
+      <c r="B157" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="2:2" ht="18">
+      <c r="B158" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="159" spans="2:2" ht="18">
+      <c r="B159" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="160" spans="2:2" ht="18">
+      <c r="B160" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="161" spans="2:2" ht="18">
+      <c r="B161" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="162" spans="2:2" ht="18">
+      <c r="B162" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="163" spans="2:2" ht="18">
+      <c r="B163" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="164" spans="2:2" ht="18">
+      <c r="B164" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="165" spans="2:2" ht="18">
+      <c r="B165" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="166" spans="2:2" ht="18">
+      <c r="B166" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="167" spans="2:2" ht="18">
+      <c r="B167" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="2:2" ht="18">
+      <c r="B168" s="3">
+        <v>44409</v>
+      </c>
+    </row>
+    <row r="169" spans="2:2" ht="18">
+      <c r="B169" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="170" spans="2:2" ht="18">
+      <c r="B170" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="171" spans="2:2" ht="18">
+      <c r="B171" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="172" spans="2:2" ht="18">
+      <c r="B172" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="173" spans="2:2" ht="18">
+      <c r="B173" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="174" spans="2:2" ht="18">
+      <c r="B174" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="175" spans="2:2" ht="18">
+      <c r="B175" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="176" spans="2:2" ht="18">
+      <c r="B176" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="177" spans="2:2" ht="18">
+      <c r="B177" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="178" spans="2:2" ht="18">
+      <c r="B178" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="179" spans="2:2" ht="18">
+      <c r="B179" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="180" spans="2:2" ht="18">
+      <c r="B180" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="2:2" ht="18">
+      <c r="B181" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="182" spans="2:2" ht="18">
+      <c r="B182" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="183" spans="2:2" ht="18">
+      <c r="B183" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="184" spans="2:2" ht="18">
+      <c r="B184" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="185" spans="2:2" ht="18">
+      <c r="B185" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="186" spans="2:2" ht="18">
+      <c r="B186" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="187" spans="2:2" ht="18">
+      <c r="B187" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="188" spans="2:2" ht="18">
+      <c r="B188" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="189" spans="2:2" ht="18">
+      <c r="B189" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="190" spans="2:2" ht="18">
+      <c r="B190" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="191" spans="2:2" ht="18">
+      <c r="B191" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="192" spans="2:2" ht="18">
+      <c r="B192" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="193" spans="2:2" ht="18">
+      <c r="B193" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="194" spans="2:2" ht="18">
+      <c r="B194" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="195" spans="2:2" ht="18">
+      <c r="B195" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="196" spans="2:2" ht="18">
+      <c r="B196" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="197" spans="2:2" ht="18">
+      <c r="B197" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="198" spans="2:2" ht="18">
+      <c r="B198" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="199" spans="2:2" ht="18">
+      <c r="B199" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="200" spans="2:2" ht="18">
+      <c r="B200" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201" spans="2:2" ht="18">
+      <c r="B201" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="202" spans="2:2" ht="18">
+      <c r="B202" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="203" spans="2:2" ht="18">
+      <c r="B203" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="204" spans="2:2" ht="18">
+      <c r="B204" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="205" spans="2:2" ht="18">
+      <c r="B205" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="206" spans="2:2" ht="18">
+      <c r="B206" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="207" spans="2:2" ht="18">
+      <c r="B207" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="208" spans="2:2" ht="18">
+      <c r="B208" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="209" spans="2:2" ht="18">
+      <c r="B209" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="210" spans="2:2" ht="18">
+      <c r="B210" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="211" spans="2:2" ht="18">
+      <c r="B211" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="212" spans="2:2" ht="18">
+      <c r="B212" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="213" spans="2:2" ht="18">
+      <c r="B213" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="214" spans="2:2" ht="18">
+      <c r="B214" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="215" spans="2:2" ht="18">
+      <c r="B215" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="216" spans="2:2" ht="18">
+      <c r="B216" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="217" spans="2:2" ht="18">
+      <c r="B217" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="218" spans="2:2" ht="18">
+      <c r="B218" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="219" spans="2:2" ht="18">
+      <c r="B219" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="220" spans="2:2" ht="18">
+      <c r="B220" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="221" spans="2:2" ht="18">
+      <c r="B221" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="222" spans="2:2" ht="18">
+      <c r="B222" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="223" spans="2:2" ht="18">
+      <c r="B223" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="224" spans="2:2" ht="18">
+      <c r="B224" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="225" spans="2:2" ht="18">
+      <c r="B225" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="226" spans="2:2" ht="18">
+      <c r="B226" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="227" spans="2:2" ht="18">
+      <c r="B227" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="228" spans="2:2" ht="18">
+      <c r="B228" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="229" spans="2:2" ht="18">
+      <c r="B229" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="230" spans="2:2" ht="18">
+      <c r="B230" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="231" spans="2:2" ht="18">
+      <c r="B231" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="232" spans="2:2" ht="18">
+      <c r="B232" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="233" spans="2:2" ht="18">
+      <c r="B233" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="234" spans="2:2" ht="18">
+      <c r="B234" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="235" spans="2:2" ht="18">
+      <c r="B235" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="236" spans="2:2" ht="18">
+      <c r="B236" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="237" spans="2:2" ht="18">
+      <c r="B237" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="238" spans="2:2" ht="18">
+      <c r="B238" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="239" spans="2:2" ht="18">
+      <c r="B239" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="240" spans="2:2" ht="18">
+      <c r="B240" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="241" spans="2:2" ht="18">
+      <c r="B241" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="242" spans="2:2" ht="18">
+      <c r="B242" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="243" spans="2:2" ht="18">
+      <c r="B243" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="244" spans="2:2" ht="18">
+      <c r="B244" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="245" spans="2:2" ht="18">
+      <c r="B245" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="246" spans="2:2" ht="18">
+      <c r="B246" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="247" spans="2:2" ht="18">
+      <c r="B247" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="248" spans="2:2" ht="18">
+      <c r="B248" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="249" spans="2:2" ht="18">
+      <c r="B249" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="250" spans="2:2" ht="18">
+      <c r="B250" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="251" spans="2:2" ht="18">
+      <c r="B251" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="252" spans="2:2" ht="18">
+      <c r="B252" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="253" spans="2:2" ht="18">
+      <c r="B253" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="254" spans="2:2" ht="18">
+      <c r="B254" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="255" spans="2:2" ht="18">
+      <c r="B255" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="256" spans="2:2" ht="18">
+      <c r="B256" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="257" spans="2:2" ht="18">
+      <c r="B257" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="258" spans="2:2" ht="18">
+      <c r="B258" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="259" spans="2:2" ht="18">
+      <c r="B259" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="260" spans="2:2" ht="18">
+      <c r="B260" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="261" spans="2:2" ht="18">
+      <c r="B261" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="262" spans="2:2" ht="18">
+      <c r="B262" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="263" spans="2:2" ht="18">
+      <c r="B263" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="264" spans="2:2" ht="18">
+      <c r="B264" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="265" spans="2:2" ht="18">
+      <c r="B265" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="266" spans="2:2" ht="18">
+      <c r="B266" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="267" spans="2:2" ht="18">
+      <c r="B267" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="268" spans="2:2" ht="18">
+      <c r="B268" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="269" spans="2:2" ht="18">
+      <c r="B269" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="270" spans="2:2" ht="18">
+      <c r="B270" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="271" spans="2:2" ht="18">
+      <c r="B271" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="272" spans="2:2" ht="18">
+      <c r="B272" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="273" spans="2:2" ht="18">
+      <c r="B273" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="274" spans="2:2" ht="18">
+      <c r="B274" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="275" spans="2:2" ht="18">
+      <c r="B275" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="276" spans="2:2" ht="18">
+      <c r="B276" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="277" spans="2:2" ht="18">
+      <c r="B277" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="278" spans="2:2" ht="18">
+      <c r="B278" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="279" spans="2:2" ht="18">
+      <c r="B279" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="280" spans="2:2" ht="18">
+      <c r="B280" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="281" spans="2:2" ht="18">
+      <c r="B281" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="282" spans="2:2" ht="18">
+      <c r="B282" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="283" spans="2:2" ht="18">
+      <c r="B283" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="284" spans="2:2" ht="18">
+      <c r="B284" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="285" spans="2:2" ht="18">
+      <c r="B285" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="286" spans="2:2" ht="18">
+      <c r="B286" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="287" spans="2:2" ht="18">
+      <c r="B287" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="288" spans="2:2" ht="18">
+      <c r="B288" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="289" spans="2:2" ht="18">
+      <c r="B289" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="290" spans="2:2" ht="18">
+      <c r="B290" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="291" spans="2:2" ht="18">
+      <c r="B291" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="292" spans="2:2" ht="18">
+      <c r="B292" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="293" spans="2:2" ht="18">
+      <c r="B293" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="294" spans="2:2" ht="18">
+      <c r="B294" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="295" spans="2:2" ht="18">
+      <c r="B295" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="296" spans="2:2" ht="18">
+      <c r="B296" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="297" spans="2:2" ht="18">
+      <c r="B297" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="298" spans="2:2" ht="18">
+      <c r="B298" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="299" spans="2:2" ht="18">
+      <c r="B299" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="300" spans="2:2" ht="18">
+      <c r="B300" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="302" spans="2:2" ht="18">
+      <c r="B302" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="303" spans="2:2" ht="18">
+      <c r="B303" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="304" spans="2:2" ht="18">
+      <c r="B304" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="305" spans="2:2" ht="18">
+      <c r="B305" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="306" spans="2:2" ht="18">
+      <c r="B306" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="307" spans="2:2" ht="18">
+      <c r="B307" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="308" spans="2:2" ht="18">
+      <c r="B308" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="309" spans="2:2" ht="18">
+      <c r="B309" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="310" spans="2:2" ht="18">
+      <c r="B310" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="311" spans="2:2" ht="18">
+      <c r="B311" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="312" spans="2:2" ht="18">
+      <c r="B312" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="313" spans="2:2" ht="18">
+      <c r="B313" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="314" spans="2:2" ht="18">
+      <c r="B314" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="315" spans="2:2" ht="18">
+      <c r="B315" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="316" spans="2:2" ht="18">
+      <c r="B316" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="317" spans="2:2" ht="18">
+      <c r="B317" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="318" spans="2:2" ht="18">
+      <c r="B318" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="319" spans="2:2" ht="18">
+      <c r="B319" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="320" spans="2:2" ht="18">
+      <c r="B320" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="321" spans="2:2" ht="18">
+      <c r="B321" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="322" spans="2:2" ht="18">
+      <c r="B322" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="323" spans="2:2" ht="18">
+      <c r="B323" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="324" spans="2:2" ht="18">
+      <c r="B324" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="325" spans="2:2" ht="18">
+      <c r="B325" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="326" spans="2:2" ht="18">
+      <c r="B326" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="327" spans="2:2" ht="18">
+      <c r="B327" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="328" spans="2:2" ht="18">
+      <c r="B328" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="329" spans="2:2" ht="18">
+      <c r="B329" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="330" spans="2:2" ht="18">
+      <c r="B330" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="331" spans="2:2" ht="18">
+      <c r="B331" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="332" spans="2:2" ht="18">
+      <c r="B332" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="333" spans="2:2" ht="18">
+      <c r="B333" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="334" spans="2:2" ht="18">
+      <c r="B334" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="335" spans="2:2" ht="18">
+      <c r="B335" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="336" spans="2:2" ht="18">
+      <c r="B336" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="337" spans="1:2" ht="18">
+      <c r="B337" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="338" spans="1:2" ht="18">
+      <c r="B338" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="339" spans="1:2" ht="18">
+      <c r="B339" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="340" spans="1:2" ht="18">
+      <c r="B340" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="341" spans="1:2" ht="18">
+      <c r="B341" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="342" spans="1:2" ht="18">
+      <c r="B342" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="343" spans="1:2" ht="18">
+      <c r="B343" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="344" spans="1:2" ht="18">
+      <c r="B344" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="345" spans="1:2" ht="18">
+      <c r="B345" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="346" spans="1:2" ht="18">
+      <c r="B346" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="347" spans="1:2" ht="18">
+      <c r="B347" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="348" spans="1:2" ht="18">
+      <c r="B348" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="349" spans="1:2" ht="18">
+      <c r="B349" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="350" spans="1:2" ht="18">
+      <c r="B350" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="351" spans="1:2" ht="18">
+      <c r="B351" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="352" spans="1:2" ht="18">
+      <c r="A352" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <customSheetViews>
+    <customSheetView guid="{42B17E81-1F77-D241-BD50-864917389C19}">
+      <selection activeCell="F329" sqref="F329"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+  </customSheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2DE7426-1857-914B-857F-0DD5503E94DC}">
   <dimension ref="A1:N349"/>
   <sheetViews>
-    <sheetView topLeftCell="A152" workbookViewId="0">
-      <selection activeCell="F175" sqref="F175"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C337" sqref="C337"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5084,7 +7251,7 @@
     <row r="274" spans="2:7" ht="18">
       <c r="B274" s="1"/>
       <c r="E274" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="275" spans="2:7" ht="18">
@@ -5181,7 +7348,7 @@
     <row r="285" spans="2:7" ht="18">
       <c r="B285" s="1"/>
       <c r="E285" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="286" spans="2:7" ht="18">
@@ -5280,7 +7447,7 @@
     <row r="296" spans="2:7" ht="18">
       <c r="B296" s="1"/>
       <c r="E296" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="297" spans="2:7" ht="18">
@@ -5379,7 +7546,7 @@
     <row r="307" spans="2:7" ht="18">
       <c r="B307" s="1"/>
       <c r="E307" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="308" spans="2:7" ht="18">
@@ -5708,15 +7875,21 @@
       </c>
     </row>
   </sheetData>
+  <customSheetViews>
+    <customSheetView guid="{42B17E81-1F77-D241-BD50-864917389C19}" topLeftCell="A37">
+      <selection activeCell="C337" sqref="C337"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+  </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6ECD5DD-B09F-3C40-8156-ABB84AC0BF4C}">
   <dimension ref="B3:O346"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A91" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B173" sqref="B173"/>
     </sheetView>
   </sheetViews>
@@ -8278,6 +10451,12 @@
       <c r="B346" s="1"/>
     </row>
   </sheetData>
+  <customSheetViews>
+    <customSheetView guid="{42B17E81-1F77-D241-BD50-864917389C19}" scale="90" topLeftCell="A91">
+      <selection activeCell="B173" sqref="B173"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+  </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>